<commit_message>
Vollständige Vorarbeit, nur bei Aufgabe d ?? & das eigentliche einzeichnen der Punkte ist nicht vorhanden & der Lineare Vergleich
</commit_message>
<xml_diff>
--- a/k_means_vorarbeit.xlsx
+++ b/k_means_vorarbeit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Studium\FH-SWF\6. Semster\IoT\Praktikum\Praktikum1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0BFAAF-55C0-4BC4-8908-5EC5BEAF7A21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AD94FD-DD3F-476B-9F00-89F2376380AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="15390" xr2:uid="{B97834B6-E166-467E-9822-D14E888C8722}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t>Temperatur</t>
   </si>
@@ -70,6 +70,36 @@
   </si>
   <si>
     <t>Clustering mittels k-mean Algorithmus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aufgabe b) </t>
+  </si>
+  <si>
+    <t>Aufgabe a)</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aufgabe c) </t>
+  </si>
+  <si>
+    <t>Vergleich zum 2. Durchlauf</t>
+  </si>
+  <si>
+    <t>Zeigt keine Verbesserung, da Werte weiter auseinander laufen würden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aufgabe d) </t>
+  </si>
+  <si>
+    <t>Wenn die Mittelwertegeben sind würde ich die Centroiden, anhand dessen verteilen, da dies ein gutes Maß dafür wäre.</t>
+  </si>
+  <si>
+    <t>?????????</t>
   </si>
 </sst>
 </file>
@@ -141,20 +171,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -235,7 +273,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>k_means_Algorithmus!$B$5</c:f>
+              <c:f>k_means_Algorithmus!$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -316,7 +354,7 @@
           </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>k_means_Algorithmus!$A$6:$A$17</c:f>
+              <c:f>k_means_Algorithmus!$A$7:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -361,7 +399,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>k_means_Algorithmus!$B$6:$B$17</c:f>
+              <c:f>k_means_Algorithmus!$B$7:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -664,7 +702,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>k_means_Algorithmus!$B$5</c:f>
+              <c:f>k_means_Algorithmus!$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1039,7 +1077,7 @@
           </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>k_means_Algorithmus!$A$6:$A$17</c:f>
+              <c:f>k_means_Algorithmus!$A$7:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1084,7 +1122,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>k_means_Algorithmus!$B$6:$B$17</c:f>
+              <c:f>k_means_Algorithmus!$B$7:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1379,7 +1417,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>k_means_Algorithmus!$B$46</c:f>
+              <c:f>k_means_Algorithmus!$B$47</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1456,7 +1494,7 @@
           </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>k_means_Algorithmus!$A$47:$A$58</c:f>
+              <c:f>k_means_Algorithmus!$A$48:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1501,7 +1539,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>k_means_Algorithmus!$B$47:$B$58</c:f>
+              <c:f>k_means_Algorithmus!$B$48:$B$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1795,7 +1833,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>k_means_Algorithmus!$B$46</c:f>
+              <c:f>k_means_Algorithmus!$B$47</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2162,7 +2200,7 @@
           </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>k_means_Algorithmus!$A$47:$A$58</c:f>
+              <c:f>k_means_Algorithmus!$A$48:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2207,7 +2245,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>k_means_Algorithmus!$B$47:$B$58</c:f>
+              <c:f>k_means_Algorithmus!$B$48:$B$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2501,7 +2539,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>k_means_Algorithmus!$B$87</c:f>
+              <c:f>k_means_Algorithmus!$B$88</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2798,7 +2836,7 @@
           </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>k_means_Algorithmus!$A$88:$A$99</c:f>
+              <c:f>k_means_Algorithmus!$A$89:$A$100</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2843,7 +2881,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>k_means_Algorithmus!$B$88:$B$99</c:f>
+              <c:f>k_means_Algorithmus!$B$89:$B$100</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3026,6 +3064,586 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="550488912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>k_means_Algorithmus!$B$105</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sensorwerte</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-E30E-4D54-9B4C-F405381E83C5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-E30E-4D54-9B4C-F405381E83C5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:marker>
+              <c:symbol val="star"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-E30E-4D54-9B4C-F405381E83C5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-E30E-4D54-9B4C-F405381E83C5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-E30E-4D54-9B4C-F405381E83C5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-E30E-4D54-9B4C-F405381E83C5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-E30E-4D54-9B4C-F405381E83C5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:marker>
+              <c:symbol val="star"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent6"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-E30E-4D54-9B4C-F405381E83C5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-E30E-4D54-9B4C-F405381E83C5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:xVal>
+            <c:numRef>
+              <c:f>k_means_Algorithmus!$A$106:$A$119</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>k_means_Algorithmus!$B$106:$B$119</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>31.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E30E-4D54-9B4C-F405381E83C5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="504821392"/>
+        <c:axId val="504817456"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="504821392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="504817456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="504817456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="504821392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
@@ -3276,6 +3894,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5341,6 +5999,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5862,13 +7036,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5898,13 +7072,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5936,13 +7110,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>223836</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>742949</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5972,13 +7146,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>357188</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>14288</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6010,13 +7184,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>519112</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>119061</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>99</xdr:row>
+      <xdr:row>100</xdr:row>
       <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6037,6 +7211,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Diagramm 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C1F9E7C-29C4-488E-AF52-8A019195523D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6342,187 +7552,180 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4295456-A300-42D3-AAE5-B18407093BE0}">
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:H131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1">
-        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>2</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B8" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>2</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B9" s="2">
         <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" s="1">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1">
-        <v>38</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="1">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="1">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>9</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B16" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
         <v>10</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B17" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>10</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B18" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="5"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="B23" s="7"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>1</v>
-      </c>
-      <c r="B25" s="2">
-        <v>5</v>
-      </c>
-      <c r="C25" s="2">
-        <f>(A25-$A$27)^2+(B25-$B$27)^2</f>
-        <v>170</v>
-      </c>
-      <c r="D25" s="2">
-        <f>(A25-$A$35)^2+(B25-$B$35)^2</f>
-        <v>370</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C26" s="2">
-        <f>(A26-$A$27)^2+(B26-$B$27)^2</f>
-        <v>256</v>
+        <f>(A26-$A$28)^2+(B26-$B$28)^2</f>
+        <v>170</v>
       </c>
       <c r="D26" s="2">
-        <f>(A26-$A$35)^2+(B26-$B$35)^2</f>
-        <v>464</v>
+        <f>(A26-$A$36)^2+(B26-$B$36)^2</f>
+        <v>370</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -6530,143 +7733,143 @@
         <v>2</v>
       </c>
       <c r="B27" s="2">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C27" s="2">
-        <f>(A27-$A$27)^2+(B27-$B$27)^2</f>
-        <v>0</v>
+        <f>(A27-$A$28)^2+(B27-$B$28)^2</f>
+        <v>256</v>
       </c>
       <c r="D27" s="2">
-        <f>(A27-$A$35)^2+(B27-$B$35)^2</f>
-        <v>80</v>
+        <f>(A27-$A$36)^2+(B27-$B$36)^2</f>
+        <v>464</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B28" s="2">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C28" s="2">
-        <f>(A28-$A$27)^2+(B28-$B$27)^2</f>
-        <v>50</v>
+        <f>(A28-$A$28)^2+(B28-$B$28)^2</f>
+        <v>0</v>
       </c>
       <c r="D28" s="2">
-        <f>(A28-$A$35)^2+(B28-$B$35)^2</f>
-        <v>58</v>
+        <f>(A28-$A$36)^2+(B28-$B$36)^2</f>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
+        <v>3</v>
+      </c>
+      <c r="B29" s="2">
+        <v>25</v>
+      </c>
+      <c r="C29" s="2">
+        <f>(A29-$A$28)^2+(B29-$B$28)^2</f>
+        <v>50</v>
+      </c>
+      <c r="D29" s="2">
+        <f>(A29-$A$36)^2+(B29-$B$36)^2</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
         <v>4</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B30" s="2">
         <v>10</v>
       </c>
-      <c r="C29" s="2">
-        <f t="shared" ref="C29:C36" si="0">(A29-$A$27)^2+(B29-$B$27)^2</f>
+      <c r="C30" s="2">
+        <f t="shared" ref="C30:C37" si="0">(A30-$A$28)^2+(B30-$B$28)^2</f>
         <v>68</v>
       </c>
-      <c r="D29" s="2">
-        <f t="shared" ref="D29:D36" si="1">(A29-$A$35)^2+(B29-$B$35)^2</f>
+      <c r="D30" s="2">
+        <f t="shared" ref="D30:D37" si="1">(A30-$A$36)^2+(B30-$B$36)^2</f>
         <v>180</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
         <v>5</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B31" s="3">
         <v>38</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C31" s="3">
         <f t="shared" si="0"/>
         <v>409</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D31" s="3">
         <f t="shared" si="1"/>
         <v>281</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
         <v>6</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B32" s="2">
         <v>1</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>305</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D32" s="2">
         <f t="shared" si="1"/>
         <v>457</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
         <v>7</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B33" s="3">
         <v>22</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C33" s="3">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D33" s="3">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
         <v>8</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B34" s="2">
         <v>8</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C34" s="2">
         <f t="shared" si="0"/>
         <v>136</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D34" s="2">
         <f t="shared" si="1"/>
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
         <v>9</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B35" s="2">
         <v>12</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C35" s="2">
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D35" s="2">
         <f t="shared" si="1"/>
         <v>101</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
-        <v>10</v>
-      </c>
-      <c r="B35" s="3">
-        <v>22</v>
-      </c>
-      <c r="C35" s="3">
-        <f t="shared" ref="C35" si="2">(A35-$A$27)^2+(B35-$B$27)^2</f>
-        <v>80</v>
-      </c>
-      <c r="D35" s="3">
-        <f t="shared" ref="D35" si="3">(A35-$A$35)^2+(B35-$B$35)^2</f>
-        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -6674,641 +7877,1002 @@
         <v>10</v>
       </c>
       <c r="B36" s="3">
+        <v>22</v>
+      </c>
+      <c r="C36" s="3">
+        <f t="shared" ref="C36" si="2">(A36-$A$28)^2+(B36-$B$28)^2</f>
+        <v>80</v>
+      </c>
+      <c r="D36" s="3">
+        <f t="shared" ref="D36" si="3">(A36-$A$36)^2+(B36-$B$36)^2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>10</v>
+      </c>
+      <c r="B37" s="3">
         <v>42</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C37" s="3">
         <f t="shared" si="0"/>
         <v>640</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D37" s="3">
         <f t="shared" si="1"/>
         <v>400</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="5"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="B40" s="7"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B42">
-        <f>ROUNDUP((SUM(A25,A26,A27,A29,A31,A33,A34)/7),1)</f>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <f>ROUNDUP((SUM(A26,A27,A28,A30,A32,A34,A35)/7),1)</f>
         <v>4.5999999999999996</v>
       </c>
-      <c r="C42">
-        <f>ROUNDUP((SUM(B25,B26,B27,B29,B31,B33,B34)/7),1)</f>
+      <c r="C43">
+        <f>ROUNDUP((SUM(B26,B27,B28,B30,B32,B34,B35)/7),1)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B44">
-        <f>ROUNDUP((SUM(A30,A32,A36)/3),1)</f>
+      <c r="B45">
+        <f>ROUNDUP((SUM(A31,A33,A37)/3),1)</f>
         <v>7.3999999999999995</v>
       </c>
-      <c r="C44">
-        <f>ROUNDUP((SUM(B30,B32,B36)/3),1)</f>
+      <c r="C45">
+        <f>ROUNDUP((SUM(B31,B33,B37)/3),1)</f>
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
-        <v>1</v>
-      </c>
-      <c r="B47" s="4">
-        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
+        <v>1</v>
+      </c>
+      <c r="B48" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
         <v>2</v>
       </c>
-      <c r="B48" s="4">
+      <c r="B49" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
-        <f>B42</f>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <f>B43</f>
         <v>4.5999999999999996</v>
       </c>
-      <c r="B49" s="2">
-        <f>C42</f>
+      <c r="B50" s="2">
+        <f>C43</f>
         <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
-        <v>3</v>
-      </c>
-      <c r="B50" s="4">
-        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B51" s="4">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B52" s="4">
-        <v>38</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B53" s="4">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B54" s="4">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B55" s="4">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
+        <v>8</v>
+      </c>
+      <c r="B56" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
         <v>9</v>
       </c>
-      <c r="B56" s="4">
+      <c r="B57" s="4">
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="3">
-        <f>B44</f>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <f>B45</f>
         <v>7.3999999999999995</v>
       </c>
-      <c r="B57" s="3">
-        <f>C44</f>
+      <c r="B58" s="3">
+        <f>C45</f>
         <v>34</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
         <v>10</v>
       </c>
-      <c r="B58" s="4">
+      <c r="B59" s="4">
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B62" s="5"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="B63" s="7"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
-        <v>1</v>
-      </c>
-      <c r="B64" s="2">
-        <v>5</v>
-      </c>
-      <c r="C64" s="2">
-        <f>(A64-$A$66)^2+(B64-$B$66)^2</f>
-        <v>21.959999999999997</v>
-      </c>
-      <c r="D64" s="2">
-        <f>(A64-$A$74)^2+(B64-$B$74)^2</f>
-        <v>881.96</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B65" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C65" s="2">
-        <f t="shared" ref="C65:C75" si="4">(A65-$A$66)^2+(B65-$B$66)^2</f>
-        <v>42.76</v>
+        <f>(A65-$A$67)^2+(B65-$B$67)^2</f>
+        <v>21.959999999999997</v>
       </c>
       <c r="D65" s="2">
-        <f t="shared" ref="D65:D75" si="5">(A65-$A$74)^2+(B65-$B$74)^2</f>
-        <v>1053.1600000000001</v>
+        <f>(A65-$A$75)^2+(B65-$B$75)^2</f>
+        <v>881.96</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <f>B42</f>
+        <v>2</v>
+      </c>
+      <c r="B66" s="2">
+        <v>2</v>
+      </c>
+      <c r="C66" s="2">
+        <f t="shared" ref="C66:C76" si="4">(A66-$A$67)^2+(B66-$B$67)^2</f>
+        <v>42.76</v>
+      </c>
+      <c r="D66" s="2">
+        <f t="shared" ref="D66:D76" si="5">(A66-$A$75)^2+(B66-$B$75)^2</f>
+        <v>1053.1600000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <f>B43</f>
         <v>4.5999999999999996</v>
       </c>
-      <c r="B66" s="2">
-        <f>C42</f>
+      <c r="B67" s="2">
+        <f>C43</f>
         <v>8</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C67" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D66" s="2">
+      <c r="D67" s="2">
         <f t="shared" si="5"/>
         <v>683.84</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="3">
         <v>3</v>
       </c>
-      <c r="B67" s="3">
+      <c r="B68" s="3">
         <v>25</v>
       </c>
-      <c r="C67" s="3">
+      <c r="C68" s="3">
         <f t="shared" si="4"/>
         <v>291.56</v>
       </c>
-      <c r="D67" s="3">
+      <c r="D68" s="3">
         <f t="shared" si="5"/>
         <v>100.36</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
         <v>4</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B69" s="2">
         <v>10</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C69" s="2">
         <f t="shared" si="4"/>
         <v>4.3599999999999994</v>
       </c>
-      <c r="D68" s="2">
+      <c r="D69" s="2">
         <f t="shared" si="5"/>
         <v>587.55999999999995</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
         <v>5</v>
       </c>
-      <c r="B69" s="3">
+      <c r="B70" s="3">
         <v>38</v>
       </c>
-      <c r="C69" s="3">
+      <c r="C70" s="3">
         <f t="shared" si="4"/>
         <v>900.16</v>
       </c>
-      <c r="D69" s="3">
+      <c r="D70" s="3">
         <f t="shared" si="5"/>
         <v>21.759999999999998</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
         <v>6</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B71" s="2">
         <v>1</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C71" s="2">
         <f t="shared" si="4"/>
         <v>50.96</v>
       </c>
-      <c r="D70" s="2">
+      <c r="D71" s="2">
         <f t="shared" si="5"/>
         <v>1090.96</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="3">
         <v>7</v>
       </c>
-      <c r="B71" s="3">
+      <c r="B72" s="3">
         <v>22</v>
       </c>
-      <c r="C71" s="3">
+      <c r="C72" s="3">
         <f t="shared" si="4"/>
         <v>201.76</v>
       </c>
-      <c r="D71" s="3">
+      <c r="D72" s="3">
         <f t="shared" si="5"/>
         <v>144.16</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
         <v>8</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B73" s="2">
         <v>8</v>
       </c>
-      <c r="C72" s="2">
+      <c r="C73" s="2">
         <f t="shared" si="4"/>
         <v>11.560000000000002</v>
       </c>
-      <c r="D72" s="2">
+      <c r="D73" s="2">
         <f t="shared" si="5"/>
         <v>676.36</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
         <v>9</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B74" s="2">
         <v>12</v>
       </c>
-      <c r="C73" s="2">
+      <c r="C74" s="2">
         <f t="shared" si="4"/>
         <v>35.36</v>
       </c>
-      <c r="D73" s="2">
+      <c r="D74" s="2">
         <f t="shared" si="5"/>
         <v>486.56</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="3">
-        <f>B44</f>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="3">
+        <f>B45</f>
         <v>7.3999999999999995</v>
       </c>
-      <c r="B74" s="3">
-        <f>C44</f>
+      <c r="B75" s="3">
+        <f>C45</f>
         <v>34</v>
       </c>
-      <c r="C74" s="3">
+      <c r="C75" s="3">
         <f t="shared" si="4"/>
         <v>683.84</v>
       </c>
-      <c r="D74" s="3">
+      <c r="D75" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="3">
         <v>10</v>
       </c>
-      <c r="B75" s="3">
+      <c r="B76" s="3">
         <v>42</v>
       </c>
-      <c r="C75" s="3">
+      <c r="C76" s="3">
         <f t="shared" si="4"/>
         <v>1185.1600000000001</v>
       </c>
-      <c r="D75" s="3">
+      <c r="D76" s="3">
         <f t="shared" si="5"/>
         <v>70.760000000000005</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B79" s="5"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+      <c r="B80" s="7"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B82" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B82" s="1">
-        <f>ROUNDUP((SUM(A64,A65,A68,A70,A72,A73)/6),1)</f>
+      <c r="C82" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="1">
+        <f>ROUNDUP((SUM(A65,A66,A69,A71,A73,A74)/6),1)</f>
         <v>5</v>
       </c>
-      <c r="C82" s="1">
-        <f>ROUNDUP((SUM(B64,B65,B68,B70,B72,B73)/6),1)</f>
+      <c r="C83" s="1">
+        <f>ROUNDUP((SUM(B65,B66,B69,B71,B73,B74)/6),1)</f>
         <v>6.3999999999999995</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-    </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B84" s="1">
-        <f>ROUNDUP((SUM(A67,A69,A71,A75)/4),1)</f>
+      <c r="B85" s="1">
+        <f>ROUNDUP((SUM(A68,A70,A72,A76)/4),1)</f>
         <v>6.3</v>
       </c>
-      <c r="C84" s="1">
-        <f>ROUNDUP((SUM(B67,B69,B71,B75)/4),1)</f>
+      <c r="C85" s="1">
+        <f>ROUNDUP((SUM(B68,B70,B72,B76)/4),1)</f>
         <v>31.8</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B88" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C88" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="D88" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="2">
-        <v>1</v>
-      </c>
-      <c r="B88" s="2">
-        <v>5</v>
-      </c>
-      <c r="C88" s="2">
-        <f>(A88-$A$90)^2+(B88-$B$90)^2</f>
-        <v>17.959999999999997</v>
-      </c>
-      <c r="D88" s="2">
-        <f>(A88-$A$98)^2+(B88-$B$98)^2</f>
-        <v>746.33</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B89" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C89" s="2">
-        <f t="shared" ref="C89:C99" si="6">(A89-$A$90)^2+(B89-$B$90)^2</f>
-        <v>28.359999999999996</v>
+        <f>(A89-$A$91)^2+(B89-$B$91)^2</f>
+        <v>17.959999999999997</v>
       </c>
       <c r="D89" s="2">
-        <f t="shared" ref="D89:D99" si="7">(A89-$A$98)^2+(B89-$B$98)^2</f>
-        <v>906.53000000000009</v>
+        <f>(A89-$A$99)^2+(B89-$B$99)^2</f>
+        <v>746.33</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <f>B82</f>
+        <v>2</v>
+      </c>
+      <c r="B90" s="2">
+        <v>2</v>
+      </c>
+      <c r="C90" s="2">
+        <f t="shared" ref="C90:C100" si="6">(A90-$A$91)^2+(B90-$B$91)^2</f>
+        <v>28.359999999999996</v>
+      </c>
+      <c r="D90" s="2">
+        <f t="shared" ref="D90:D100" si="7">(A90-$A$99)^2+(B90-$B$99)^2</f>
+        <v>906.53000000000009</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <f>B83</f>
         <v>5</v>
       </c>
-      <c r="B90" s="2">
-        <f>C82</f>
+      <c r="B91" s="2">
+        <f>C83</f>
         <v>6.3999999999999995</v>
       </c>
-      <c r="C90" s="2">
+      <c r="C91" s="2">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="D90" s="2">
+      <c r="D91" s="2">
         <f t="shared" si="7"/>
         <v>646.85000000000014</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="3">
         <v>3</v>
       </c>
-      <c r="B91" s="3">
+      <c r="B92" s="3">
         <v>25</v>
       </c>
-      <c r="C91" s="3">
+      <c r="C92" s="3">
         <f t="shared" si="6"/>
         <v>349.96000000000004</v>
       </c>
-      <c r="D91" s="3">
+      <c r="D92" s="3">
         <f t="shared" si="7"/>
         <v>57.13000000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
         <v>4</v>
       </c>
-      <c r="B92" s="2">
+      <c r="B93" s="2">
         <v>10</v>
       </c>
-      <c r="C92" s="2">
+      <c r="C93" s="2">
         <f t="shared" si="6"/>
         <v>13.960000000000004</v>
       </c>
-      <c r="D92" s="2">
+      <c r="D93" s="2">
         <f t="shared" si="7"/>
         <v>480.53000000000003</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="3">
         <v>5</v>
       </c>
-      <c r="B93" s="3">
+      <c r="B94" s="3">
         <v>38</v>
       </c>
-      <c r="C93" s="3">
+      <c r="C94" s="3">
         <f t="shared" si="6"/>
         <v>998.56000000000006</v>
       </c>
-      <c r="D93" s="3">
+      <c r="D94" s="3">
         <f t="shared" si="7"/>
         <v>40.129999999999988</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
         <v>6</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B95" s="2">
         <v>1</v>
       </c>
-      <c r="C94" s="2">
+      <c r="C95" s="2">
         <f t="shared" si="6"/>
         <v>30.159999999999993</v>
       </c>
-      <c r="D94" s="2">
+      <c r="D95" s="2">
         <f t="shared" si="7"/>
         <v>948.73000000000013</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="3">
         <v>7</v>
       </c>
-      <c r="B95" s="3">
+      <c r="B96" s="3">
         <v>22</v>
       </c>
-      <c r="C95" s="3">
+      <c r="C96" s="3">
         <f t="shared" si="6"/>
         <v>247.36000000000004</v>
       </c>
-      <c r="D95" s="3">
+      <c r="D96" s="3">
         <f t="shared" si="7"/>
         <v>96.530000000000015</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
         <v>8</v>
       </c>
-      <c r="B96" s="2">
+      <c r="B97" s="2">
         <v>8</v>
       </c>
-      <c r="C96" s="2">
+      <c r="C97" s="2">
         <f t="shared" si="6"/>
         <v>11.560000000000002</v>
       </c>
-      <c r="D96" s="2">
+      <c r="D97" s="2">
         <f t="shared" si="7"/>
         <v>569.33000000000004</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
         <v>9</v>
       </c>
-      <c r="B97" s="2">
+      <c r="B98" s="2">
         <v>12</v>
       </c>
-      <c r="C97" s="2">
+      <c r="C98" s="2">
         <f t="shared" si="6"/>
         <v>47.360000000000007</v>
       </c>
-      <c r="D97" s="2">
+      <c r="D98" s="2">
         <f t="shared" si="7"/>
         <v>399.33000000000004</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="3">
-        <f>B84</f>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="3">
+        <f>B85</f>
         <v>6.3</v>
       </c>
-      <c r="B98" s="3">
-        <f>C84</f>
+      <c r="B99" s="3">
+        <f>C85</f>
         <v>31.8</v>
       </c>
-      <c r="C98" s="3">
+      <c r="C99" s="3">
         <f t="shared" si="6"/>
         <v>646.85000000000014</v>
       </c>
-      <c r="D98" s="3">
+      <c r="D99" s="3">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="3">
         <v>10</v>
       </c>
-      <c r="B99" s="3">
+      <c r="B100" s="3">
         <v>42</v>
       </c>
-      <c r="C99" s="3">
+      <c r="C100" s="3">
         <f t="shared" si="6"/>
         <v>1292.3600000000001</v>
       </c>
-      <c r="D99" s="3">
+      <c r="D100" s="3">
         <f t="shared" si="7"/>
         <v>117.72999999999999</v>
       </c>
     </row>
+    <row r="103" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A103" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="2">
+        <v>1</v>
+      </c>
+      <c r="B106" s="2">
+        <v>5</v>
+      </c>
+      <c r="C106" s="2">
+        <f>(A106-$A$91)^2+(B106-$B$91)^2</f>
+        <v>17.959999999999997</v>
+      </c>
+      <c r="D106" s="2">
+        <f>(A106-$A$99)^2+(B106-$B$99)^2</f>
+        <v>746.33</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="2">
+        <v>2</v>
+      </c>
+      <c r="B107" s="2">
+        <v>2</v>
+      </c>
+      <c r="C107" s="2">
+        <f t="shared" ref="C107:C119" si="8">(A107-$A$91)^2+(B107-$B$91)^2</f>
+        <v>28.359999999999996</v>
+      </c>
+      <c r="D107" s="2">
+        <f t="shared" ref="D107:D119" si="9">(A107-$A$99)^2+(B107-$B$99)^2</f>
+        <v>906.53000000000009</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="2">
+        <f>B83</f>
+        <v>5</v>
+      </c>
+      <c r="B108" s="2">
+        <f>C83</f>
+        <v>6.3999999999999995</v>
+      </c>
+      <c r="C108" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="D108" s="2">
+        <f t="shared" si="9"/>
+        <v>646.85000000000014</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="3">
+        <v>3</v>
+      </c>
+      <c r="B109" s="3">
+        <v>25</v>
+      </c>
+      <c r="C109" s="3">
+        <f t="shared" si="8"/>
+        <v>349.96000000000004</v>
+      </c>
+      <c r="D109" s="3">
+        <f t="shared" si="9"/>
+        <v>57.13000000000001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
+        <v>4</v>
+      </c>
+      <c r="B110" s="2">
+        <v>10</v>
+      </c>
+      <c r="C110" s="2">
+        <f t="shared" si="8"/>
+        <v>13.960000000000004</v>
+      </c>
+      <c r="D110" s="2">
+        <f t="shared" si="9"/>
+        <v>480.53000000000003</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="3">
+        <v>5</v>
+      </c>
+      <c r="B111" s="3">
+        <v>38</v>
+      </c>
+      <c r="C111" s="3">
+        <f t="shared" si="8"/>
+        <v>998.56000000000006</v>
+      </c>
+      <c r="D111" s="3">
+        <f t="shared" si="9"/>
+        <v>40.129999999999988</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="2">
+        <v>6</v>
+      </c>
+      <c r="B112" s="2">
+        <v>1</v>
+      </c>
+      <c r="C112" s="2">
+        <f t="shared" si="8"/>
+        <v>30.159999999999993</v>
+      </c>
+      <c r="D112" s="2">
+        <f t="shared" si="9"/>
+        <v>948.73000000000013</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="3">
+        <v>7</v>
+      </c>
+      <c r="B113" s="3">
+        <v>22</v>
+      </c>
+      <c r="C113" s="3">
+        <f t="shared" si="8"/>
+        <v>247.36000000000004</v>
+      </c>
+      <c r="D113" s="3">
+        <f t="shared" si="9"/>
+        <v>96.530000000000015</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="2">
+        <v>8</v>
+      </c>
+      <c r="B114" s="2">
+        <v>8</v>
+      </c>
+      <c r="C114" s="2">
+        <f t="shared" si="8"/>
+        <v>11.560000000000002</v>
+      </c>
+      <c r="D114" s="2">
+        <f t="shared" si="9"/>
+        <v>569.33000000000004</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="2">
+        <v>9</v>
+      </c>
+      <c r="B115" s="2">
+        <v>12</v>
+      </c>
+      <c r="C115" s="2">
+        <f t="shared" si="8"/>
+        <v>47.360000000000007</v>
+      </c>
+      <c r="D115" s="2">
+        <f t="shared" si="9"/>
+        <v>399.33000000000004</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="3">
+        <f>B85</f>
+        <v>6.3</v>
+      </c>
+      <c r="B116" s="3">
+        <f>C85</f>
+        <v>31.8</v>
+      </c>
+      <c r="C116" s="3">
+        <f t="shared" si="8"/>
+        <v>646.85000000000014</v>
+      </c>
+      <c r="D116" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="3">
+        <v>10</v>
+      </c>
+      <c r="B117" s="3">
+        <v>42</v>
+      </c>
+      <c r="C117" s="3">
+        <f t="shared" si="8"/>
+        <v>1292.3600000000001</v>
+      </c>
+      <c r="D117" s="3">
+        <f t="shared" si="9"/>
+        <v>117.72999999999999</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="2">
+        <v>8</v>
+      </c>
+      <c r="B118" s="2">
+        <v>18</v>
+      </c>
+      <c r="C118" s="2">
+        <f t="shared" si="8"/>
+        <v>143.56000000000003</v>
+      </c>
+      <c r="D118" s="2">
+        <f t="shared" si="9"/>
+        <v>193.33000000000004</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="3">
+        <v>10</v>
+      </c>
+      <c r="B119" s="3">
+        <v>30</v>
+      </c>
+      <c r="C119" s="3">
+        <f t="shared" si="8"/>
+        <v>581.96</v>
+      </c>
+      <c r="D119" s="3">
+        <f t="shared" si="9"/>
+        <v>16.930000000000003</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A122" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="1"/>
+      <c r="B124" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D124" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E124" s="7"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B125" s="1">
+        <f>ROUNDUP((SUM(A106,A107,A110,A112,A114,A115,A118)/7),1)</f>
+        <v>5.5</v>
+      </c>
+      <c r="C125" s="1">
+        <f>ROUNDUP((SUM(B106,B107,B110,B112,B114,B115,B118)/7),1)</f>
+        <v>8</v>
+      </c>
+      <c r="D125" s="11">
+        <f>(B125-B83)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E125" s="11">
+        <f>(C125-C83)</f>
+        <v>1.6000000000000005</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B126" s="1">
+        <f>ROUNDUP((SUM(A109,A111,A113,A117,A119)/5),1)</f>
+        <v>7</v>
+      </c>
+      <c r="C126" s="1">
+        <f>ROUNDUP((SUM(B109,B111,B113,B117,B119)/5),1)</f>
+        <v>31.4</v>
+      </c>
+      <c r="D126">
+        <f>B126-B85</f>
+        <v>0.70000000000000018</v>
+      </c>
+      <c r="E126">
+        <f>C126-C85</f>
+        <v>-0.40000000000000213</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B128" s="12"/>
+      <c r="C128" s="12"/>
+      <c r="D128" s="12"/>
+      <c r="E128" s="12"/>
+    </row>
+    <row r="130" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A130" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B130" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A131" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B131" s="10"/>
+      <c r="C131" s="10"/>
+      <c r="D131" s="10"/>
+      <c r="E131" s="10"/>
+      <c r="F131" s="10"/>
+      <c r="G131" s="10"/>
+      <c r="H131" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A79:B79"/>
+  <mergeCells count="8">
+    <mergeCell ref="D124:E124"/>
+    <mergeCell ref="A128:E128"/>
+    <mergeCell ref="A131:H131"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A80:B80"/>
     <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>